<commit_message>
removing unnecessary backup file
this is why i should learn visual studio instead of using notepad++ for everything
</commit_message>
<xml_diff>
--- a/Admin Files/Cosmetic Changes.xlsx
+++ b/Admin Files/Cosmetic Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6002EB7E-64B8-46ED-8368-59A39F06DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73205B-25AE-4531-84D2-5838B7CE5953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-20640" yWindow="8715" windowWidth="24525" windowHeight="15495" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -125,6 +123,12 @@
   </si>
   <si>
     <t>Low tier, but will make the game environment much funner</t>
+  </si>
+  <si>
+    <t>LETS GOOOOOOO FOOTBALL MINIGAME WITH MUSHROOMS YEAHHH</t>
+  </si>
+  <si>
+    <t>Low (very high)</t>
   </si>
 </sst>
 </file>
@@ -162,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,17 +189,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -525,7 +539,7 @@
     <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -539,7 +553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -567,7 +581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -581,7 +595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -595,7 +609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -609,7 +623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -623,7 +637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -637,7 +651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -645,13 +659,16 @@
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
adding to cosmetic file
</commit_message>
<xml_diff>
--- a/Admin Files/Cosmetic Changes.xlsx
+++ b/Admin Files/Cosmetic Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Speck\git\strung-along\Admin Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73205B-25AE-4531-84D2-5838B7CE5953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6412F7B-6A1C-4F17-B8AE-36F1008CAA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="8715" windowWidth="24525" windowHeight="15495" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -122,13 +122,40 @@
     <t>Should show upon game start</t>
   </si>
   <si>
-    <t>Low tier, but will make the game environment much funner</t>
-  </si>
-  <si>
-    <t>LETS GOOOOOOO FOOTBALL MINIGAME WITH MUSHROOMS YEAHHH</t>
-  </si>
-  <si>
     <t>Low (very high)</t>
+  </si>
+  <si>
+    <t>Add colliders to stage poles</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Add colliders under mushrooms/tables</t>
+  </si>
+  <si>
+    <t>Anything that a player can walk undeneath should be blocked</t>
+  </si>
+  <si>
+    <t>Make strings look like visual strings</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>You know</t>
+  </si>
+  <si>
+    <t>Create actual assets for the anchor points</t>
+  </si>
+  <si>
+    <t>Skye/Lauren</t>
+  </si>
+  <si>
+    <t>Could get spicy with them and add effects like, tilting as you move, pulling up when the character jumps</t>
+  </si>
+  <si>
+    <t>Low tier, but will make the game environment much funner (LETS GOOOOOOO FOOTBALL MINIGAME WITH MUSHROOMS YEAHHH)</t>
   </si>
 </sst>
 </file>
@@ -166,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,27 +216,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +562,7 @@
     <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -553,8 +576,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -567,8 +590,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -581,8 +604,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -595,8 +618,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -609,8 +632,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -623,8 +646,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -637,8 +660,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -651,25 +674,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -679,6 +701,60 @@
         <v>19</v>
       </c>
       <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ticked off and added some tasks to cosmetic fixes
</commit_message>
<xml_diff>
--- a/Admin Files/Cosmetic Changes.xlsx
+++ b/Admin Files/Cosmetic Changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6412F7B-6A1C-4F17-B8AE-36F1008CAA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD11B70-6FB6-4EC1-9B94-517895D7FAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Low tier, but will make the game environment much funner (LETS GOOOOOOO FOOTBALL MINIGAME WITH MUSHROOMS YEAHHH)</t>
+  </si>
+  <si>
+    <t>Opening screen</t>
+  </si>
+  <si>
+    <t>Shows on startup.</t>
+  </si>
+  <si>
+    <t>Closing screen</t>
+  </si>
+  <si>
+    <t>Show on gameover or when you complete</t>
+  </si>
+  <si>
+    <t>Fix boxes moving through each other when grabbed</t>
+  </si>
+  <si>
+    <t>Hard cause I know to move them we disabled the collider, but has to be fixed</t>
   </si>
 </sst>
 </file>
@@ -179,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +207,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -233,6 +257,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,127 +661,169 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added changes to the task tracking document
</commit_message>
<xml_diff>
--- a/Admin Files/Cosmetic Changes.xlsx
+++ b/Admin Files/Cosmetic Changes.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD11B70-6FB6-4EC1-9B94-517895D7FAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932F8073-FE81-4050-98C8-4353B6C5E1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MinorTasksWeek2" sheetId="1" r:id="rId1"/>
+    <sheet name="MinorTasksWeek3" sheetId="3" r:id="rId2"/>
+    <sheet name="MajorTasks" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Particle effects on goals</t>
   </si>
@@ -174,6 +176,24 @@
   </si>
   <si>
     <t>Hard cause I know to move them we disabled the collider, but has to be fixed</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Dropdown, started, havent started, done needs testing, done testing finished</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Potentailly track time task, estimated time vs actual time taken</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Consider tagging bugs</t>
   </si>
 </sst>
 </file>
@@ -217,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -240,11 +260,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -262,6 +291,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F2CD5D-B7CE-4B02-AEAB-57CB269396F3}">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +620,283 @@
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71EE719-A9DF-4A98-A156-8D0839D934B9}">
+  <dimension ref="B2:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -689,23 +998,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="9" t="s">
+    <row r="9" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>27</v>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>7</v>
@@ -714,120 +1023,106 @@
         <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F60F0-D37C-48A6-81DA-136DEAEF3BF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>